<commit_message>
$  git config --global user.email fuguai-24h365d@outlook.jp $  git config --global user.name Assamteactc
</commit_message>
<xml_diff>
--- a/data/ID参照表.xlsx
+++ b/data/ID参照表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\github\kc-fp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fugua\github\kc-fp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F38B7F-EA54-481F-98A8-6448763004F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D71BD13-EE45-449F-9050-303E974F35A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="50565" windowHeight="21840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="検索表" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="id" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">艦名!$A$1:$C$358</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">艦名!$A$1:$E$358</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="835">
   <si>
     <t>艦名</t>
     <rPh sb="0" eb="2">
@@ -2553,13 +2553,33 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Atlanta</t>
+    <t>磯風乙改</t>
+    <rPh sb="2" eb="3">
+      <t>オツ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Atlanta改</t>
-    <rPh sb="7" eb="8">
-      <t>カイ</t>
+    <t>浜風乙改</t>
+    <rPh sb="2" eb="3">
+      <t>オツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>秋月</t>
+    <rPh sb="0" eb="2">
+      <t>アキヅキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>白露改二</t>
+    <rPh sb="0" eb="2">
+      <t>シラツユ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カイニ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2911,14 +2931,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Z722"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="5.625" customWidth="1"/>
-    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="5.59765625" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" customWidth="1"/>
     <col min="7" max="7" width="62.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2944,19 +2964,19 @@
     </row>
     <row r="3" spans="2:26">
       <c r="B3" s="1" t="s">
-        <v>831</v>
+        <v>395</v>
       </c>
       <c r="C3" s="1">
         <f>IF(B3&lt;&gt;"",VLOOKUP(B3,艦名!A:B,2,FALSE),"")</f>
-        <v>597</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>IF(B3&lt;&gt;"",VLOOKUP(B3,艦名!A:C,3,FALSE),"")</f>
-        <v>CL</v>
+        <v>DD</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>IF(B3&lt;&gt;"",VLOOKUP(B3,艦名!A:E,5,FALSE),"")</f>
-        <v>アトランタ級</v>
+        <v>綾波型</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>91</v>
@@ -2968,19 +2988,19 @@
     </row>
     <row r="4" spans="2:26">
       <c r="B4" s="1" t="s">
-        <v>832</v>
+        <v>514</v>
       </c>
       <c r="C4" s="1">
         <f>IF(B4&lt;&gt;"",VLOOKUP(B4,艦名!A:B,2,FALSE),"")</f>
-        <v>696</v>
+        <v>233</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>IF(B4&lt;&gt;"",VLOOKUP(B4,艦名!A:C,3,FALSE),"")</f>
-        <v>CL</v>
+        <v>DD</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>IF(B4&lt;&gt;"",VLOOKUP(B4,艦名!A:E,5,FALSE),"")</f>
-        <v>アトランタ級</v>
+        <v>綾波型</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>121</v>
@@ -2989,20 +3009,28 @@
         <f>IF(G4&lt;&gt;"",VLOOKUP(G4,装備名!A:B,2,FALSE),"")</f>
         <v>295</v>
       </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="2:26">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="str">
+      <c r="B5" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="C5" s="1">
         <f>IF(B5&lt;&gt;"",VLOOKUP(B5,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>407</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>IF(B5&lt;&gt;"",VLOOKUP(B5,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E5" s="1" t="str">
         <f>IF(B5&lt;&gt;"",VLOOKUP(B5,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>綾波型</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>176</v>
@@ -3011,6 +3039,12 @@
         <f>IF(G5&lt;&gt;"",VLOOKUP(G5,装備名!A:B,2,FALSE),"")</f>
         <v>229</v>
       </c>
+      <c r="K5">
+        <v>36</v>
+      </c>
+      <c r="L5">
+        <v>122</v>
+      </c>
       <c r="N5">
         <v>566</v>
       </c>
@@ -3034,18 +3068,20 @@
       </c>
     </row>
     <row r="6" spans="2:26">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="str">
+      <c r="B6" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C6" s="1">
         <f>IF(B6&lt;&gt;"",VLOOKUP(B6,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>IF(B6&lt;&gt;"",VLOOKUP(B6,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E6" s="1" t="str">
         <f>IF(B6&lt;&gt;"",VLOOKUP(B6,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>暁型</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>84</v>
@@ -3054,6 +3090,12 @@
         <f>IF(G6&lt;&gt;"",VLOOKUP(G6,装備名!A:B,2,FALSE),"")</f>
         <v>308</v>
       </c>
+      <c r="K6">
+        <v>167</v>
+      </c>
+      <c r="L6">
+        <v>145</v>
+      </c>
       <c r="N6">
         <v>567</v>
       </c>
@@ -3077,18 +3119,20 @@
       </c>
     </row>
     <row r="7" spans="2:26">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="str">
+      <c r="B7" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C7" s="1">
         <f>IF(B7&lt;&gt;"",VLOOKUP(B7,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>236</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>IF(B7&lt;&gt;"",VLOOKUP(B7,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>IF(B7&lt;&gt;"",VLOOKUP(B7,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>暁型</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>742</v>
@@ -3097,6 +3141,12 @@
         <f>IF(G7&lt;&gt;"",VLOOKUP(G7,装備名!A:B,2,FALSE),"")</f>
         <v>313</v>
       </c>
+      <c r="K7">
+        <v>170</v>
+      </c>
+      <c r="L7">
+        <v>243</v>
+      </c>
       <c r="N7">
         <v>568</v>
       </c>
@@ -3120,18 +3170,20 @@
       </c>
     </row>
     <row r="8" spans="2:26">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="str">
+      <c r="B8" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C8" s="1">
         <f>IF(B8&lt;&gt;"",VLOOKUP(B8,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>414</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>IF(B8&lt;&gt;"",VLOOKUP(B8,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E8" s="1" t="str">
         <f>IF(B8&lt;&gt;"",VLOOKUP(B8,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>朝潮型</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>88</v>
@@ -3140,6 +3192,12 @@
         <f>IF(G8&lt;&gt;"",VLOOKUP(G8,装備名!A:B,2,FALSE),"")</f>
         <v>366</v>
       </c>
+      <c r="K8">
+        <v>233</v>
+      </c>
+      <c r="L8">
+        <v>294</v>
+      </c>
       <c r="O8">
         <v>628</v>
       </c>
@@ -3157,18 +3215,20 @@
       </c>
     </row>
     <row r="9" spans="2:26">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="str">
+      <c r="B9" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C9" s="1">
         <f>IF(B9&lt;&gt;"",VLOOKUP(B9,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>328</v>
       </c>
       <c r="D9" s="1" t="str">
         <f>IF(B9&lt;&gt;"",VLOOKUP(B9,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E9" s="1" t="str">
         <f>IF(B9&lt;&gt;"",VLOOKUP(B9,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>朝潮型</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>87</v>
@@ -3177,6 +3237,12 @@
         <f>IF(G9&lt;&gt;"",VLOOKUP(G9,装備名!A:B,2,FALSE),"")</f>
         <v>267</v>
       </c>
+      <c r="K9">
+        <v>236</v>
+      </c>
+      <c r="L9">
+        <v>344</v>
+      </c>
       <c r="O9">
         <v>629</v>
       </c>
@@ -3194,18 +3260,20 @@
       </c>
     </row>
     <row r="10" spans="2:26">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="str">
+      <c r="B10" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C10" s="1">
         <f>IF(B10&lt;&gt;"",VLOOKUP(B10,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>167</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>IF(B10&lt;&gt;"",VLOOKUP(B10,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E10" s="1" t="str">
         <f>IF(B10&lt;&gt;"",VLOOKUP(B10,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>陽炎型</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>89</v>
@@ -3214,6 +3282,12 @@
         <f>IF(G10&lt;&gt;"",VLOOKUP(G10,装備名!A:B,2,FALSE),"")</f>
         <v>266</v>
       </c>
+      <c r="K10">
+        <v>312</v>
+      </c>
+      <c r="L10">
+        <v>363</v>
+      </c>
       <c r="O10">
         <v>681</v>
       </c>
@@ -3228,18 +3302,20 @@
       </c>
     </row>
     <row r="11" spans="2:26">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="str">
+      <c r="B11" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C11" s="1">
         <f>IF(B11&lt;&gt;"",VLOOKUP(B11,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>320</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>IF(B11&lt;&gt;"",VLOOKUP(B11,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>IF(B11&lt;&gt;"",VLOOKUP(B11,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>陽炎型</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>90</v>
@@ -3248,6 +3324,12 @@
         <f>IF(G11&lt;&gt;"",VLOOKUP(G11,装備名!A:B,2,FALSE),"")</f>
         <v>63</v>
       </c>
+      <c r="K11">
+        <v>320</v>
+      </c>
+      <c r="L11">
+        <v>369</v>
+      </c>
       <c r="O11">
         <v>689</v>
       </c>
@@ -3262,18 +3344,20 @@
       </c>
     </row>
     <row r="12" spans="2:26">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="str">
+      <c r="B12" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C12" s="1">
         <f>IF(B12&lt;&gt;"",VLOOKUP(B12,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>557</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>IF(B12&lt;&gt;"",VLOOKUP(B12,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>IF(B12&lt;&gt;"",VLOOKUP(B12,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>陽炎型</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>120</v>
@@ -3282,6 +3366,12 @@
         <f>IF(G12&lt;&gt;"",VLOOKUP(G12,装備名!A:B,2,FALSE),"")</f>
         <v>294</v>
       </c>
+      <c r="K12">
+        <v>328</v>
+      </c>
+      <c r="L12">
+        <v>425</v>
+      </c>
       <c r="O12">
         <v>692</v>
       </c>
@@ -3296,18 +3386,20 @@
       </c>
     </row>
     <row r="13" spans="2:26">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="str">
+      <c r="B13" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C13" s="1">
         <f>IF(B13&lt;&gt;"",VLOOKUP(B13,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>170</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>IF(B13&lt;&gt;"",VLOOKUP(B13,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E13" s="1" t="str">
         <f>IF(B13&lt;&gt;"",VLOOKUP(B13,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>陽炎型</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>122</v>
@@ -3316,6 +3408,12 @@
         <f>IF(G13&lt;&gt;"",VLOOKUP(G13,装備名!A:B,2,FALSE),"")</f>
         <v>297</v>
       </c>
+      <c r="K13">
+        <v>407</v>
+      </c>
+      <c r="L13">
+        <v>457</v>
+      </c>
       <c r="S13">
         <v>324</v>
       </c>
@@ -3327,18 +3425,20 @@
       </c>
     </row>
     <row r="14" spans="2:26">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="str">
+      <c r="B14" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C14" s="1">
         <f>IF(B14&lt;&gt;"",VLOOKUP(B14,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>312</v>
       </c>
       <c r="D14" s="1" t="str">
         <f>IF(B14&lt;&gt;"",VLOOKUP(B14,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E14" s="1" t="str">
         <f>IF(B14&lt;&gt;"",VLOOKUP(B14,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>陽炎型</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>172</v>
@@ -3347,6 +3447,12 @@
         <f>IF(G14&lt;&gt;"",VLOOKUP(G14,装備名!A:B,2,FALSE),"")</f>
         <v>293</v>
       </c>
+      <c r="K14">
+        <v>414</v>
+      </c>
+      <c r="L14">
+        <v>471</v>
+      </c>
       <c r="S14">
         <v>325</v>
       </c>
@@ -3358,18 +3464,20 @@
       </c>
     </row>
     <row r="15" spans="2:26">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="str">
+      <c r="B15" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C15" s="1">
         <f>IF(B15&lt;&gt;"",VLOOKUP(B15,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>558</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>IF(B15&lt;&gt;"",VLOOKUP(B15,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>IF(B15&lt;&gt;"",VLOOKUP(B15,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>陽炎型</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>74</v>
@@ -3378,6 +3486,12 @@
         <f>IF(G15&lt;&gt;"",VLOOKUP(G15,装備名!A:B,2,FALSE),"")</f>
         <v>282</v>
       </c>
+      <c r="K15">
+        <v>527</v>
+      </c>
+      <c r="L15">
+        <v>473</v>
+      </c>
       <c r="S15">
         <v>344</v>
       </c>
@@ -3389,18 +3503,20 @@
       </c>
     </row>
     <row r="16" spans="2:26">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="str">
+      <c r="B16" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="C16" s="1">
         <f>IF(B16&lt;&gt;"",VLOOKUP(B16,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>527</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>IF(B16&lt;&gt;"",VLOOKUP(B16,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>IF(B16&lt;&gt;"",VLOOKUP(B16,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>夕雲型</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>45</v>
@@ -3409,6 +3525,12 @@
         <f>IF(G16&lt;&gt;"",VLOOKUP(G16,装備名!A:B,2,FALSE),"")</f>
         <v>50</v>
       </c>
+      <c r="K16">
+        <v>557</v>
+      </c>
+      <c r="L16">
+        <v>476</v>
+      </c>
       <c r="S16">
         <v>345</v>
       </c>
@@ -3420,18 +3542,20 @@
       </c>
     </row>
     <row r="17" spans="2:26">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="str">
+      <c r="B17" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="C17" s="1">
         <f>IF(B17&lt;&gt;"",VLOOKUP(B17,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>686</v>
       </c>
       <c r="D17" s="1" t="str">
         <f>IF(B17&lt;&gt;"",VLOOKUP(B17,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E17" s="1" t="str">
         <f>IF(B17&lt;&gt;"",VLOOKUP(B17,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>夕雲型</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>48</v>
@@ -3439,6 +3563,12 @@
       <c r="H17" s="1">
         <f>IF(G17&lt;&gt;"",VLOOKUP(G17,装備名!A:B,2,FALSE),"")</f>
         <v>90</v>
+      </c>
+      <c r="K17">
+        <v>558</v>
+      </c>
+      <c r="L17">
+        <v>578</v>
       </c>
       <c r="S17">
         <v>349</v>
@@ -3471,6 +3601,9 @@
         <f>IF(G18&lt;&gt;"",VLOOKUP(G18,装備名!A:B,2,FALSE),"")</f>
         <v>310</v>
       </c>
+      <c r="K18">
+        <v>686</v>
+      </c>
       <c r="S18">
         <v>359</v>
       </c>
@@ -3482,18 +3615,20 @@
       </c>
     </row>
     <row r="19" spans="2:26">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="str">
+      <c r="B19" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C19" s="1">
         <f>IF(B19&lt;&gt;"",VLOOKUP(B19,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>421</v>
       </c>
       <c r="D19" s="1" t="str">
         <f>IF(B19&lt;&gt;"",VLOOKUP(B19,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>IF(B19&lt;&gt;"",VLOOKUP(B19,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>秋月型</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>40</v>
@@ -3606,18 +3741,20 @@
       </c>
     </row>
     <row r="23" spans="2:26">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="str">
+      <c r="B23" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C23" s="1">
         <f>IF(B23&lt;&gt;"",VLOOKUP(B23,艦名!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>497</v>
       </c>
       <c r="D23" s="1" t="str">
         <f>IF(B23&lt;&gt;"",VLOOKUP(B23,艦名!A:C,3,FALSE),"")</f>
-        <v/>
+        <v>DD</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>IF(B23&lt;&gt;"",VLOOKUP(B23,艦名!A:E,5,FALSE),"")</f>
-        <v/>
+        <v>白露型</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>49</v>
@@ -17848,11 +17985,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Z5:Z40">
-    <sortCondition ref="Z5"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K4:K18">
+    <sortCondition ref="K4"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17864,7 +18002,7 @@
       <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="62" bestFit="1" customWidth="1"/>
   </cols>
@@ -20909,15 +21047,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C9A11E-B107-4104-863F-861C0A8C9DF4}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E358"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C332" sqref="C332"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="30.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="30.19921875" style="2" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
@@ -20936,7 +21075,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" hidden="1">
       <c r="A2" s="2" t="s">
         <v>384</v>
       </c>
@@ -20954,7 +21093,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" hidden="1">
       <c r="A3" s="2" t="s">
         <v>385</v>
       </c>
@@ -20972,7 +21111,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" hidden="1">
       <c r="A4" s="2" t="s">
         <v>386</v>
       </c>
@@ -20990,7 +21129,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" hidden="1">
       <c r="A5" s="2" t="s">
         <v>387</v>
       </c>
@@ -21008,7 +21147,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" hidden="1">
       <c r="A6" s="2" t="s">
         <v>388</v>
       </c>
@@ -21026,7 +21165,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" hidden="1">
       <c r="A7" s="2" t="s">
         <v>389</v>
       </c>
@@ -21044,7 +21183,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" hidden="1">
       <c r="A8" s="2" t="s">
         <v>390</v>
       </c>
@@ -21062,7 +21201,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" hidden="1">
       <c r="A9" s="2" t="s">
         <v>391</v>
       </c>
@@ -21080,7 +21219,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" hidden="1">
       <c r="A10" s="2" t="s">
         <v>392</v>
       </c>
@@ -21098,7 +21237,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" hidden="1">
       <c r="A11" s="2" t="s">
         <v>393</v>
       </c>
@@ -21116,7 +21255,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" hidden="1">
       <c r="A12" s="2" t="s">
         <v>394</v>
       </c>
@@ -21134,7 +21273,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" hidden="1">
       <c r="A13" s="2" t="s">
         <v>395</v>
       </c>
@@ -21152,7 +21291,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" hidden="1">
       <c r="A14" s="2" t="s">
         <v>396</v>
       </c>
@@ -21170,7 +21309,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" hidden="1">
       <c r="A15" s="2" t="s">
         <v>397</v>
       </c>
@@ -21188,7 +21327,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" hidden="1">
       <c r="A16" s="2" t="s">
         <v>398</v>
       </c>
@@ -21206,7 +21345,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" hidden="1">
       <c r="A17" s="2" t="s">
         <v>399</v>
       </c>
@@ -21224,7 +21363,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" hidden="1">
       <c r="A18" s="2" t="s">
         <v>400</v>
       </c>
@@ -21242,7 +21381,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" hidden="1">
       <c r="A19" s="2" t="s">
         <v>401</v>
       </c>
@@ -21260,7 +21399,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" hidden="1">
       <c r="A20" s="2" t="s">
         <v>402</v>
       </c>
@@ -21278,7 +21417,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" hidden="1">
       <c r="A21" s="2" t="s">
         <v>403</v>
       </c>
@@ -21296,7 +21435,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" hidden="1">
       <c r="A22" s="2" t="s">
         <v>404</v>
       </c>
@@ -21314,7 +21453,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" hidden="1">
       <c r="A23" s="2" t="s">
         <v>405</v>
       </c>
@@ -21332,7 +21471,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" hidden="1">
       <c r="A24" s="2" t="s">
         <v>406</v>
       </c>
@@ -21350,7 +21489,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" hidden="1">
       <c r="A25" s="2" t="s">
         <v>407</v>
       </c>
@@ -21368,7 +21507,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" hidden="1">
       <c r="A26" s="2" t="s">
         <v>408</v>
       </c>
@@ -21386,7 +21525,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" hidden="1">
       <c r="A27" s="2" t="s">
         <v>409</v>
       </c>
@@ -21404,7 +21543,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" hidden="1">
       <c r="A28" s="2" t="s">
         <v>410</v>
       </c>
@@ -21422,7 +21561,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" hidden="1">
       <c r="A29" s="2" t="s">
         <v>411</v>
       </c>
@@ -21440,7 +21579,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" hidden="1">
       <c r="A30" s="2" t="s">
         <v>412</v>
       </c>
@@ -21458,7 +21597,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" hidden="1">
       <c r="A31" s="2" t="s">
         <v>413</v>
       </c>
@@ -21476,7 +21615,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" hidden="1">
       <c r="A32" s="2" t="s">
         <v>414</v>
       </c>
@@ -21494,7 +21633,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" hidden="1">
       <c r="A33" s="2" t="s">
         <v>415</v>
       </c>
@@ -21512,7 +21651,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" hidden="1">
       <c r="A34" s="2" t="s">
         <v>416</v>
       </c>
@@ -21530,7 +21669,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" hidden="1">
       <c r="A35" s="2" t="s">
         <v>417</v>
       </c>
@@ -21548,7 +21687,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" hidden="1">
       <c r="A36" s="2" t="s">
         <v>418</v>
       </c>
@@ -21566,7 +21705,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" hidden="1">
       <c r="A37" s="2" t="s">
         <v>419</v>
       </c>
@@ -21584,7 +21723,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" hidden="1">
       <c r="A38" s="2" t="s">
         <v>420</v>
       </c>
@@ -21602,7 +21741,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" hidden="1">
       <c r="A39" s="2" t="s">
         <v>421</v>
       </c>
@@ -21620,7 +21759,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" hidden="1">
       <c r="A40" s="2" t="s">
         <v>422</v>
       </c>
@@ -21638,7 +21777,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" hidden="1">
       <c r="A41" s="2" t="s">
         <v>423</v>
       </c>
@@ -21656,7 +21795,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" hidden="1">
       <c r="A42" s="2" t="s">
         <v>424</v>
       </c>
@@ -21710,7 +21849,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" hidden="1">
       <c r="A45" s="2" t="s">
         <v>427</v>
       </c>
@@ -21728,7 +21867,7 @@
         <v>島風型</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" hidden="1">
       <c r="A46" s="2" t="s">
         <v>428</v>
       </c>
@@ -21746,7 +21885,7 @@
         <v>天龍型</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" hidden="1">
       <c r="A47" s="2" t="s">
         <v>429</v>
       </c>
@@ -21764,7 +21903,7 @@
         <v>天龍型</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" hidden="1">
       <c r="A48" s="2" t="s">
         <v>430</v>
       </c>
@@ -21782,7 +21921,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" hidden="1">
       <c r="A49" s="2" t="s">
         <v>431</v>
       </c>
@@ -21800,7 +21939,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" hidden="1">
       <c r="A50" s="2" t="s">
         <v>432</v>
       </c>
@@ -21818,7 +21957,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" hidden="1">
       <c r="A51" s="2" t="s">
         <v>433</v>
       </c>
@@ -21836,7 +21975,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" hidden="1">
       <c r="A52" s="2" t="s">
         <v>434</v>
       </c>
@@ -21854,7 +21993,7 @@
         <v>重雷装巡洋艦</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" hidden="1">
       <c r="A53" s="2" t="s">
         <v>435</v>
       </c>
@@ -21872,7 +22011,7 @@
         <v>重雷装巡洋艦</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" hidden="1">
       <c r="A54" s="2" t="s">
         <v>436</v>
       </c>
@@ -21890,7 +22029,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" hidden="1">
       <c r="A55" s="2" t="s">
         <v>437</v>
       </c>
@@ -21980,7 +22119,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" hidden="1">
       <c r="A60" s="2" t="s">
         <v>442</v>
       </c>
@@ -21998,7 +22137,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" hidden="1">
       <c r="A61" s="2" t="s">
         <v>443</v>
       </c>
@@ -22016,7 +22155,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" hidden="1">
       <c r="A62" s="2" t="s">
         <v>444</v>
       </c>
@@ -22034,7 +22173,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" hidden="1">
       <c r="A63" s="2" t="s">
         <v>445</v>
       </c>
@@ -22052,7 +22191,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" hidden="1">
       <c r="A64" s="2" t="s">
         <v>446</v>
       </c>
@@ -22070,7 +22209,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" hidden="1">
       <c r="A65" s="2" t="s">
         <v>447</v>
       </c>
@@ -22088,7 +22227,7 @@
         <v>夕張型</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" hidden="1">
       <c r="A66" s="2" t="s">
         <v>448</v>
       </c>
@@ -22106,7 +22245,7 @@
         <v>重雷装巡洋艦</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" hidden="1">
       <c r="A67" s="2" t="s">
         <v>449</v>
       </c>
@@ -22124,7 +22263,7 @@
         <v>重雷装巡洋艦</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" hidden="1">
       <c r="A68" s="2" t="s">
         <v>450</v>
       </c>
@@ -22142,7 +22281,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" hidden="1">
       <c r="A69" s="2" t="s">
         <v>451</v>
       </c>
@@ -22160,7 +22299,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" hidden="1">
       <c r="A70" s="2" t="s">
         <v>452</v>
       </c>
@@ -22178,7 +22317,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" hidden="1">
       <c r="A71" s="2" t="s">
         <v>453</v>
       </c>
@@ -22196,7 +22335,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" hidden="1">
       <c r="A72" s="2" t="s">
         <v>454</v>
       </c>
@@ -22214,7 +22353,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" hidden="1">
       <c r="A73" s="2" t="s">
         <v>455</v>
       </c>
@@ -22232,7 +22371,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" hidden="1">
       <c r="A74" s="2" t="s">
         <v>456</v>
       </c>
@@ -22250,7 +22389,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" hidden="1">
       <c r="A75" s="2" t="s">
         <v>457</v>
       </c>
@@ -22268,7 +22407,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" hidden="1">
       <c r="A76" s="2" t="s">
         <v>458</v>
       </c>
@@ -22286,7 +22425,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" hidden="1">
       <c r="A77" s="2" t="s">
         <v>459</v>
       </c>
@@ -22304,7 +22443,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" hidden="1">
       <c r="A78" s="2" t="s">
         <v>460</v>
       </c>
@@ -22322,7 +22461,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" hidden="1">
       <c r="A79" s="2" t="s">
         <v>461</v>
       </c>
@@ -22340,7 +22479,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" hidden="1">
       <c r="A80" s="2" t="s">
         <v>462</v>
       </c>
@@ -22358,7 +22497,7 @@
         <v>重雷装巡洋艦</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" hidden="1">
       <c r="A81" s="2" t="s">
         <v>463</v>
       </c>
@@ -22376,7 +22515,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" hidden="1">
       <c r="A82" s="2" t="s">
         <v>464</v>
       </c>
@@ -22394,7 +22533,7 @@
         <v>練習巡洋艦</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" hidden="1">
       <c r="A83" s="2" t="s">
         <v>465</v>
       </c>
@@ -22412,7 +22551,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" hidden="1">
       <c r="A84" s="2" t="s">
         <v>466</v>
       </c>
@@ -22430,7 +22569,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" hidden="1">
       <c r="A85" s="2" t="s">
         <v>467</v>
       </c>
@@ -22448,7 +22587,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" hidden="1">
       <c r="A86" s="2" t="s">
         <v>468</v>
       </c>
@@ -22466,7 +22605,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" hidden="1">
       <c r="A87" s="2" t="s">
         <v>469</v>
       </c>
@@ -22484,7 +22623,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" hidden="1">
       <c r="A88" s="2" t="s">
         <v>470</v>
       </c>
@@ -22502,7 +22641,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" hidden="1">
       <c r="A89" s="2" t="s">
         <v>471</v>
       </c>
@@ -22520,7 +22659,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" hidden="1">
       <c r="A90" s="2" t="s">
         <v>472</v>
       </c>
@@ -22538,7 +22677,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" hidden="1">
       <c r="A91" s="2" t="s">
         <v>473</v>
       </c>
@@ -22556,7 +22695,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" hidden="1">
       <c r="A92" s="2" t="s">
         <v>474</v>
       </c>
@@ -22574,7 +22713,7 @@
         <v>Z1型</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" hidden="1">
       <c r="A93" s="2" t="s">
         <v>475</v>
       </c>
@@ -22592,7 +22731,7 @@
         <v>Z1型</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" hidden="1">
       <c r="A94" s="2" t="s">
         <v>476</v>
       </c>
@@ -22610,7 +22749,7 @@
         <v>Z1型</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" hidden="1">
       <c r="A95" s="2" t="s">
         <v>477</v>
       </c>
@@ -22628,7 +22767,7 @@
         <v>Z1型</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" hidden="1">
       <c r="A96" s="2" t="s">
         <v>478</v>
       </c>
@@ -22646,7 +22785,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" hidden="1">
       <c r="A97" s="2" t="s">
         <v>479</v>
       </c>
@@ -22664,7 +22803,7 @@
         <v>大淀型</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" hidden="1">
       <c r="A98" s="2" t="s">
         <v>480</v>
       </c>
@@ -22682,7 +22821,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" hidden="1">
       <c r="A99" s="2" t="s">
         <v>481</v>
       </c>
@@ -22700,7 +22839,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" hidden="1">
       <c r="A100" s="2" t="s">
         <v>482</v>
       </c>
@@ -22754,7 +22893,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" hidden="1">
       <c r="A103" s="2" t="s">
         <v>485</v>
       </c>
@@ -22772,7 +22911,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" hidden="1">
       <c r="A104" s="2" t="s">
         <v>486</v>
       </c>
@@ -22790,7 +22929,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" hidden="1">
       <c r="A105" s="2" t="s">
         <v>487</v>
       </c>
@@ -22808,7 +22947,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" hidden="1">
       <c r="A106" s="2" t="s">
         <v>488</v>
       </c>
@@ -22826,7 +22965,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" hidden="1">
       <c r="A107" s="2" t="s">
         <v>489</v>
       </c>
@@ -22844,7 +22983,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" hidden="1">
       <c r="A108" s="2" t="s">
         <v>490</v>
       </c>
@@ -22862,7 +23001,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" hidden="1">
       <c r="A109" s="2" t="s">
         <v>491</v>
       </c>
@@ -22880,7 +23019,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" hidden="1">
       <c r="A110" s="2" t="s">
         <v>492</v>
       </c>
@@ -22898,7 +23037,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" hidden="1">
       <c r="A111" s="2" t="s">
         <v>493</v>
       </c>
@@ -22916,7 +23055,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" hidden="1">
       <c r="A112" s="2" t="s">
         <v>494</v>
       </c>
@@ -22934,7 +23073,7 @@
         <v>天龍型</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" hidden="1">
       <c r="A113" s="2" t="s">
         <v>495</v>
       </c>
@@ -22952,7 +23091,7 @@
         <v>天龍型</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" hidden="1">
       <c r="A114" s="2" t="s">
         <v>496</v>
       </c>
@@ -22970,7 +23109,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" hidden="1">
       <c r="A115" s="2" t="s">
         <v>497</v>
       </c>
@@ -22988,7 +23127,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" hidden="1">
       <c r="A116" s="2" t="s">
         <v>498</v>
       </c>
@@ -23006,7 +23145,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" hidden="1">
       <c r="A117" s="2" t="s">
         <v>499</v>
       </c>
@@ -23024,7 +23163,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" hidden="1">
       <c r="A118" s="2" t="s">
         <v>500</v>
       </c>
@@ -23042,7 +23181,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" hidden="1">
       <c r="A119" s="2" t="s">
         <v>501</v>
       </c>
@@ -23060,7 +23199,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" hidden="1">
       <c r="A120" s="2" t="s">
         <v>502</v>
       </c>
@@ -23078,7 +23217,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" hidden="1">
       <c r="A121" s="2" t="s">
         <v>503</v>
       </c>
@@ -23096,7 +23235,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" hidden="1">
       <c r="A122" s="2" t="s">
         <v>504</v>
       </c>
@@ -23114,7 +23253,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" hidden="1">
       <c r="A123" s="2" t="s">
         <v>505</v>
       </c>
@@ -23132,7 +23271,7 @@
         <v>川内型</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" hidden="1">
       <c r="A124" s="2" t="s">
         <v>506</v>
       </c>
@@ -23150,7 +23289,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" hidden="1">
       <c r="A125" s="2" t="s">
         <v>507</v>
       </c>
@@ -23168,7 +23307,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" hidden="1">
       <c r="A126" s="2" t="s">
         <v>508</v>
       </c>
@@ -23186,7 +23325,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" hidden="1">
       <c r="A127" s="2" t="s">
         <v>509</v>
       </c>
@@ -23204,7 +23343,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" hidden="1">
       <c r="A128" s="2" t="s">
         <v>510</v>
       </c>
@@ -23222,7 +23361,7 @@
         <v>島風型</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" hidden="1">
       <c r="A129" s="2" t="s">
         <v>511</v>
       </c>
@@ -23240,7 +23379,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" hidden="1">
       <c r="A130" s="2" t="s">
         <v>512</v>
       </c>
@@ -23258,7 +23397,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" hidden="1">
       <c r="A131" s="2" t="s">
         <v>513</v>
       </c>
@@ -23276,7 +23415,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" hidden="1">
       <c r="A132" s="2" t="s">
         <v>514</v>
       </c>
@@ -23294,7 +23433,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" hidden="1">
       <c r="A133" s="2" t="s">
         <v>515</v>
       </c>
@@ -23312,7 +23451,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" hidden="1">
       <c r="A134" s="2" t="s">
         <v>516</v>
       </c>
@@ -23330,7 +23469,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" hidden="1">
       <c r="A135" s="2" t="s">
         <v>517</v>
       </c>
@@ -23348,7 +23487,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" hidden="1">
       <c r="A136" s="2" t="s">
         <v>518</v>
       </c>
@@ -23366,7 +23505,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" hidden="1">
       <c r="A137" s="2" t="s">
         <v>519</v>
       </c>
@@ -23384,7 +23523,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" hidden="1">
       <c r="A138" s="2" t="s">
         <v>520</v>
       </c>
@@ -23402,7 +23541,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" hidden="1">
       <c r="A139" s="2" t="s">
         <v>521</v>
       </c>
@@ -23420,7 +23559,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" hidden="1">
       <c r="A140" s="2" t="s">
         <v>522</v>
       </c>
@@ -23438,7 +23577,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" hidden="1">
       <c r="A141" s="2" t="s">
         <v>523</v>
       </c>
@@ -23456,7 +23595,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" hidden="1">
       <c r="A142" s="2" t="s">
         <v>524</v>
       </c>
@@ -23474,7 +23613,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" hidden="1">
       <c r="A143" s="2" t="s">
         <v>525</v>
       </c>
@@ -23492,7 +23631,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" hidden="1">
       <c r="A144" s="2" t="s">
         <v>526</v>
       </c>
@@ -23510,7 +23649,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" hidden="1">
       <c r="A145" s="2" t="s">
         <v>527</v>
       </c>
@@ -23528,7 +23667,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" hidden="1">
       <c r="A146" s="2" t="s">
         <v>528</v>
       </c>
@@ -23654,7 +23793,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" hidden="1">
       <c r="A153" s="2" t="s">
         <v>535</v>
       </c>
@@ -23672,7 +23811,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" hidden="1">
       <c r="A154" s="2" t="s">
         <v>536</v>
       </c>
@@ -23690,7 +23829,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" hidden="1">
       <c r="A155" s="2" t="s">
         <v>537</v>
       </c>
@@ -23708,7 +23847,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" hidden="1">
       <c r="A156" s="2" t="s">
         <v>538</v>
       </c>
@@ -23726,7 +23865,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" hidden="1">
       <c r="A157" s="2" t="s">
         <v>539</v>
       </c>
@@ -23744,7 +23883,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" hidden="1">
       <c r="A158" s="2" t="s">
         <v>540</v>
       </c>
@@ -23762,7 +23901,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" hidden="1">
       <c r="A159" s="2" t="s">
         <v>541</v>
       </c>
@@ -23780,7 +23919,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" hidden="1">
       <c r="A160" s="2" t="s">
         <v>542</v>
       </c>
@@ -23798,7 +23937,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" hidden="1">
       <c r="A161" s="2" t="s">
         <v>543</v>
       </c>
@@ -23816,7 +23955,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" hidden="1">
       <c r="A162" s="2" t="s">
         <v>544</v>
       </c>
@@ -23834,7 +23973,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" hidden="1">
       <c r="A163" s="2" t="s">
         <v>545</v>
       </c>
@@ -23852,7 +23991,7 @@
         <v>夕張型</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" hidden="1">
       <c r="A164" s="2" t="s">
         <v>546</v>
       </c>
@@ -23870,7 +24009,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" hidden="1">
       <c r="A165" s="2" t="s">
         <v>547</v>
       </c>
@@ -23888,7 +24027,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" hidden="1">
       <c r="A166" s="2" t="s">
         <v>548</v>
       </c>
@@ -23906,7 +24045,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" hidden="1">
       <c r="A167" s="2" t="s">
         <v>549</v>
       </c>
@@ -23924,7 +24063,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" hidden="1">
       <c r="A168" s="2" t="s">
         <v>550</v>
       </c>
@@ -23942,7 +24081,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" hidden="1">
       <c r="A169" s="2" t="s">
         <v>551</v>
       </c>
@@ -23960,7 +24099,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" hidden="1">
       <c r="A170" s="2" t="s">
         <v>552</v>
       </c>
@@ -23978,7 +24117,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" hidden="1">
       <c r="A171" s="2" t="s">
         <v>553</v>
       </c>
@@ -23996,7 +24135,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" hidden="1">
       <c r="A172" s="2" t="s">
         <v>554</v>
       </c>
@@ -24014,7 +24153,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" hidden="1">
       <c r="A173" s="2" t="s">
         <v>555</v>
       </c>
@@ -24032,7 +24171,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" hidden="1">
       <c r="A174" s="2" t="s">
         <v>556</v>
       </c>
@@ -24050,7 +24189,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" hidden="1">
       <c r="A175" s="2" t="s">
         <v>557</v>
       </c>
@@ -24068,7 +24207,7 @@
         <v>Z1型</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" hidden="1">
       <c r="A176" s="2" t="s">
         <v>558</v>
       </c>
@@ -24086,7 +24225,7 @@
         <v>Z1型</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" hidden="1">
       <c r="A177" s="2" t="s">
         <v>559</v>
       </c>
@@ -24104,7 +24243,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" hidden="1">
       <c r="A178" s="2" t="s">
         <v>560</v>
       </c>
@@ -24122,7 +24261,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" hidden="1">
       <c r="A179" s="2" t="s">
         <v>561</v>
       </c>
@@ -24140,7 +24279,7 @@
         <v>阿賀野型</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" hidden="1">
       <c r="A180" s="2" t="s">
         <v>562</v>
       </c>
@@ -24158,7 +24297,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" hidden="1">
       <c r="A181" s="2" t="s">
         <v>563</v>
       </c>
@@ -24176,7 +24315,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" hidden="1">
       <c r="A182" s="2" t="s">
         <v>564</v>
       </c>
@@ -24194,7 +24333,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" hidden="1">
       <c r="A183" s="2" t="s">
         <v>565</v>
       </c>
@@ -24212,7 +24351,7 @@
         <v>大淀型</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" hidden="1">
       <c r="A184" s="2" t="s">
         <v>566</v>
       </c>
@@ -24230,7 +24369,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" hidden="1">
       <c r="A185" s="2" t="s">
         <v>567</v>
       </c>
@@ -24248,7 +24387,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" hidden="1">
       <c r="A186" s="2" t="s">
         <v>568</v>
       </c>
@@ -24266,7 +24405,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" hidden="1">
       <c r="A187" s="2" t="s">
         <v>569</v>
       </c>
@@ -24284,7 +24423,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" hidden="1">
       <c r="A188" s="2" t="s">
         <v>570</v>
       </c>
@@ -24338,7 +24477,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" hidden="1">
       <c r="A191" s="2" t="s">
         <v>573</v>
       </c>
@@ -24356,7 +24495,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" hidden="1">
       <c r="A192" s="2" t="s">
         <v>574</v>
       </c>
@@ -24374,7 +24513,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" hidden="1">
       <c r="A193" s="2" t="s">
         <v>575</v>
       </c>
@@ -24392,7 +24531,7 @@
         <v>練習巡洋艦</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" hidden="1">
       <c r="A194" s="2" t="s">
         <v>576</v>
       </c>
@@ -24410,7 +24549,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" hidden="1">
       <c r="A195" s="2" t="s">
         <v>577</v>
       </c>
@@ -24428,7 +24567,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" hidden="1">
       <c r="A196" s="2" t="s">
         <v>578</v>
       </c>
@@ -24446,7 +24585,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" hidden="1">
       <c r="A197" s="2" t="s">
         <v>579</v>
       </c>
@@ -24464,7 +24603,7 @@
         <v>マエストラーレ級</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" hidden="1">
       <c r="A198" s="2" t="s">
         <v>580</v>
       </c>
@@ -24482,7 +24621,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" hidden="1">
       <c r="A199" s="2" t="s">
         <v>581</v>
       </c>
@@ -24500,7 +24639,7 @@
         <v>改白露型</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" hidden="1">
       <c r="A200" s="2" t="s">
         <v>582</v>
       </c>
@@ -24518,7 +24657,7 @@
         <v>改白露型</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" hidden="1">
       <c r="A201" s="2" t="s">
         <v>583</v>
       </c>
@@ -24536,7 +24675,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" hidden="1">
       <c r="A202" s="2" t="s">
         <v>584</v>
       </c>
@@ -24554,7 +24693,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" hidden="1">
       <c r="A203" s="2" t="s">
         <v>585</v>
       </c>
@@ -24572,7 +24711,7 @@
         <v>練習巡洋艦</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" hidden="1">
       <c r="A204" s="2" t="s">
         <v>586</v>
       </c>
@@ -24590,7 +24729,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" hidden="1">
       <c r="A205" s="2" t="s">
         <v>587</v>
       </c>
@@ -24608,7 +24747,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" hidden="1">
       <c r="A206" s="2" t="s">
         <v>588</v>
       </c>
@@ -24626,7 +24765,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" hidden="1">
       <c r="A207" s="2" t="s">
         <v>589</v>
       </c>
@@ -24644,7 +24783,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" hidden="1">
       <c r="A208" s="2" t="s">
         <v>590</v>
       </c>
@@ -24662,7 +24801,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:5" hidden="1">
       <c r="A209" s="2" t="s">
         <v>591</v>
       </c>
@@ -24680,7 +24819,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:5" hidden="1">
       <c r="A210" s="2" t="s">
         <v>592</v>
       </c>
@@ -24698,7 +24837,7 @@
         <v>改白露型</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" hidden="1">
       <c r="A211" s="2" t="s">
         <v>593</v>
       </c>
@@ -24716,7 +24855,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
+    <row r="212" spans="1:5" hidden="1">
       <c r="A212" s="2" t="s">
         <v>594</v>
       </c>
@@ -24734,7 +24873,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:5" hidden="1">
       <c r="A213" s="2" t="s">
         <v>595</v>
       </c>
@@ -24752,7 +24891,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:5" hidden="1">
       <c r="A214" s="2" t="s">
         <v>596</v>
       </c>
@@ -24770,7 +24909,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:5" hidden="1">
       <c r="A215" s="2" t="s">
         <v>597</v>
       </c>
@@ -24788,7 +24927,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
+    <row r="216" spans="1:5" hidden="1">
       <c r="A216" s="2" t="s">
         <v>598</v>
       </c>
@@ -24806,7 +24945,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
+    <row r="217" spans="1:5" hidden="1">
       <c r="A217" s="2" t="s">
         <v>599</v>
       </c>
@@ -24824,7 +24963,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" hidden="1">
       <c r="A218" s="2" t="s">
         <v>600</v>
       </c>
@@ -24842,7 +24981,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" hidden="1">
       <c r="A219" s="2" t="s">
         <v>601</v>
       </c>
@@ -24860,7 +24999,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" hidden="1">
       <c r="A220" s="2" t="s">
         <v>602</v>
       </c>
@@ -24878,7 +25017,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" hidden="1">
       <c r="A221" s="2" t="s">
         <v>603</v>
       </c>
@@ -24896,7 +25035,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
+    <row r="222" spans="1:5" hidden="1">
       <c r="A222" s="2" t="s">
         <v>604</v>
       </c>
@@ -24914,7 +25053,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="223" spans="1:5">
+    <row r="223" spans="1:5" hidden="1">
       <c r="A223" s="2" t="s">
         <v>605</v>
       </c>
@@ -24932,7 +25071,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" hidden="1">
       <c r="A224" s="2" t="s">
         <v>606</v>
       </c>
@@ -24950,7 +25089,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:5" hidden="1">
       <c r="A225" s="2" t="s">
         <v>607</v>
       </c>
@@ -24968,7 +25107,7 @@
         <v>J級</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:5" hidden="1">
       <c r="A226" s="2" t="s">
         <v>608</v>
       </c>
@@ -24986,7 +25125,7 @@
         <v>Ташкент級</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" hidden="1">
       <c r="A227" s="2" t="s">
         <v>609</v>
       </c>
@@ -25004,7 +25143,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" hidden="1">
       <c r="A228" s="2" t="s">
         <v>610</v>
       </c>
@@ -25022,7 +25161,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" hidden="1">
       <c r="A229" s="2" t="s">
         <v>611</v>
       </c>
@@ -25040,7 +25179,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" hidden="1">
       <c r="A230" s="2" t="s">
         <v>612</v>
       </c>
@@ -25094,7 +25233,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" hidden="1">
       <c r="A233" s="2" t="s">
         <v>615</v>
       </c>
@@ -25112,7 +25251,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" hidden="1">
       <c r="A234" s="2" t="s">
         <v>616</v>
       </c>
@@ -25130,7 +25269,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
+    <row r="235" spans="1:5" hidden="1">
       <c r="A235" s="2" t="s">
         <v>617</v>
       </c>
@@ -25148,7 +25287,7 @@
         <v>初春型</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" hidden="1">
       <c r="A236" s="2" t="s">
         <v>618</v>
       </c>
@@ -25166,7 +25305,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" hidden="1">
       <c r="A237" s="2" t="s">
         <v>619</v>
       </c>
@@ -25184,7 +25323,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:5" hidden="1">
       <c r="A238" s="2" t="s">
         <v>620</v>
       </c>
@@ -25202,7 +25341,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
+    <row r="239" spans="1:5" hidden="1">
       <c r="A239" s="2" t="s">
         <v>621</v>
       </c>
@@ -25220,7 +25359,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:5" hidden="1">
       <c r="A240" s="2" t="s">
         <v>622</v>
       </c>
@@ -25238,7 +25377,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:5" hidden="1">
       <c r="A241" s="2" t="s">
         <v>623</v>
       </c>
@@ -25256,7 +25395,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:5" hidden="1">
       <c r="A242" s="2" t="s">
         <v>624</v>
       </c>
@@ -25274,7 +25413,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:5" hidden="1">
       <c r="A243" s="2" t="s">
         <v>625</v>
       </c>
@@ -25292,7 +25431,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
+    <row r="244" spans="1:5" hidden="1">
       <c r="A244" s="2" t="s">
         <v>626</v>
       </c>
@@ -25310,7 +25449,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:5" hidden="1">
       <c r="A245" s="2" t="s">
         <v>627</v>
       </c>
@@ -25328,7 +25467,7 @@
         <v>暁型</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:5" hidden="1">
       <c r="A246" s="2" t="s">
         <v>628</v>
       </c>
@@ -25346,7 +25485,7 @@
         <v>マエストラーレ級</v>
       </c>
     </row>
-    <row r="247" spans="1:5">
+    <row r="247" spans="1:5" hidden="1">
       <c r="A247" s="2" t="s">
         <v>629</v>
       </c>
@@ -25364,7 +25503,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="248" spans="1:5">
+    <row r="248" spans="1:5" hidden="1">
       <c r="A248" s="2" t="s">
         <v>630</v>
       </c>
@@ -25382,7 +25521,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:5" hidden="1">
       <c r="A249" s="2" t="s">
         <v>631</v>
       </c>
@@ -25400,7 +25539,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:5" hidden="1">
       <c r="A250" s="2" t="s">
         <v>632</v>
       </c>
@@ -25418,7 +25557,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:5" hidden="1">
       <c r="A251" s="2" t="s">
         <v>633</v>
       </c>
@@ -25436,7 +25575,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:5" hidden="1">
       <c r="A252" s="2" t="s">
         <v>634</v>
       </c>
@@ -25454,7 +25593,7 @@
         <v>改白露型</v>
       </c>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:5" hidden="1">
       <c r="A253" s="2" t="s">
         <v>635</v>
       </c>
@@ -25472,7 +25611,7 @@
         <v>改白露型</v>
       </c>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:5" hidden="1">
       <c r="A254" s="2" t="s">
         <v>636</v>
       </c>
@@ -25526,7 +25665,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="257" spans="1:5">
+    <row r="257" spans="1:5" hidden="1">
       <c r="A257" s="2" t="s">
         <v>639</v>
       </c>
@@ -25562,7 +25701,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="259" spans="1:5">
+    <row r="259" spans="1:5" hidden="1">
       <c r="A259" s="2" t="s">
         <v>641</v>
       </c>
@@ -25598,7 +25737,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="261" spans="1:5">
+    <row r="261" spans="1:5" hidden="1">
       <c r="A261" s="2" t="s">
         <v>643</v>
       </c>
@@ -25616,7 +25755,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="262" spans="1:5">
+    <row r="262" spans="1:5" hidden="1">
       <c r="A262" s="2" t="s">
         <v>644</v>
       </c>
@@ -25634,7 +25773,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="263" spans="1:5">
+    <row r="263" spans="1:5" hidden="1">
       <c r="A263" s="2" t="s">
         <v>645</v>
       </c>
@@ -25652,7 +25791,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="264" spans="1:5">
+    <row r="264" spans="1:5" hidden="1">
       <c r="A264" s="2" t="s">
         <v>646</v>
       </c>
@@ -25670,7 +25809,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:5" hidden="1">
       <c r="A265" s="2" t="s">
         <v>647</v>
       </c>
@@ -25688,7 +25827,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="266" spans="1:5">
+    <row r="266" spans="1:5" hidden="1">
       <c r="A266" s="2" t="s">
         <v>648</v>
       </c>
@@ -25706,7 +25845,7 @@
         <v>神風型</v>
       </c>
     </row>
-    <row r="267" spans="1:5">
+    <row r="267" spans="1:5" hidden="1">
       <c r="A267" s="2" t="s">
         <v>649</v>
       </c>
@@ -25724,7 +25863,7 @@
         <v>天龍型</v>
       </c>
     </row>
-    <row r="268" spans="1:5">
+    <row r="268" spans="1:5" hidden="1">
       <c r="A268" s="2" t="s">
         <v>650</v>
       </c>
@@ -25742,7 +25881,7 @@
         <v>天龍型</v>
       </c>
     </row>
-    <row r="269" spans="1:5">
+    <row r="269" spans="1:5" hidden="1">
       <c r="A269" s="2" t="s">
         <v>651</v>
       </c>
@@ -25760,7 +25899,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="270" spans="1:5">
+    <row r="270" spans="1:5" hidden="1">
       <c r="A270" s="2" t="s">
         <v>652</v>
       </c>
@@ -25778,7 +25917,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="271" spans="1:5">
+    <row r="271" spans="1:5" hidden="1">
       <c r="A271" s="2" t="s">
         <v>653</v>
       </c>
@@ -25796,7 +25935,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="272" spans="1:5">
+    <row r="272" spans="1:5" hidden="1">
       <c r="A272" s="2" t="s">
         <v>654</v>
       </c>
@@ -25814,7 +25953,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="273" spans="1:5">
+    <row r="273" spans="1:5" hidden="1">
       <c r="A273" s="2" t="s">
         <v>655</v>
       </c>
@@ -25832,7 +25971,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="274" spans="1:5">
+    <row r="274" spans="1:5" hidden="1">
       <c r="A274" s="2" t="s">
         <v>656</v>
       </c>
@@ -25850,7 +25989,7 @@
         <v>吹雪型</v>
       </c>
     </row>
-    <row r="275" spans="1:5">
+    <row r="275" spans="1:5" hidden="1">
       <c r="A275" s="2" t="s">
         <v>657</v>
       </c>
@@ -25868,7 +26007,7 @@
         <v>長良型</v>
       </c>
     </row>
-    <row r="276" spans="1:5">
+    <row r="276" spans="1:5" hidden="1">
       <c r="A276" s="2" t="s">
         <v>658</v>
       </c>
@@ -25922,7 +26061,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="279" spans="1:5">
+    <row r="279" spans="1:5" hidden="1">
       <c r="A279" s="2" t="s">
         <v>661</v>
       </c>
@@ -25940,7 +26079,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="280" spans="1:5">
+    <row r="280" spans="1:5" hidden="1">
       <c r="A280" s="2" t="s">
         <v>662</v>
       </c>
@@ -25958,7 +26097,7 @@
         <v>白露型</v>
       </c>
     </row>
-    <row r="281" spans="1:5">
+    <row r="281" spans="1:5" hidden="1">
       <c r="A281" s="2" t="s">
         <v>663</v>
       </c>
@@ -25976,7 +26115,7 @@
         <v>Ташкент級</v>
       </c>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" hidden="1">
       <c r="A282" s="2" t="s">
         <v>664</v>
       </c>
@@ -25994,7 +26133,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="283" spans="1:5">
+    <row r="283" spans="1:5" hidden="1">
       <c r="A283" s="2" t="s">
         <v>665</v>
       </c>
@@ -26012,7 +26151,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" hidden="1">
       <c r="A284" s="2" t="s">
         <v>666</v>
       </c>
@@ -26030,7 +26169,7 @@
         <v>J級</v>
       </c>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" hidden="1">
       <c r="A285" s="2" t="s">
         <v>667</v>
       </c>
@@ -26048,7 +26187,7 @@
         <v>J級</v>
       </c>
     </row>
-    <row r="286" spans="1:5">
+    <row r="286" spans="1:5" hidden="1">
       <c r="A286" s="2" t="s">
         <v>668</v>
       </c>
@@ -26066,7 +26205,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="287" spans="1:5">
+    <row r="287" spans="1:5" hidden="1">
       <c r="A287" s="2" t="s">
         <v>669</v>
       </c>
@@ -26084,7 +26223,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" hidden="1">
       <c r="A288" s="2" t="s">
         <v>670</v>
       </c>
@@ -26102,7 +26241,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="289" spans="1:5">
+    <row r="289" spans="1:5" hidden="1">
       <c r="A289" s="2" t="s">
         <v>671</v>
       </c>
@@ -26120,7 +26259,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="290" spans="1:5">
+    <row r="290" spans="1:5" hidden="1">
       <c r="A290" s="2" t="s">
         <v>672</v>
       </c>
@@ -26138,7 +26277,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="291" spans="1:5">
+    <row r="291" spans="1:5" hidden="1">
       <c r="A291" s="2" t="s">
         <v>673</v>
       </c>
@@ -26156,7 +26295,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="292" spans="1:5">
+    <row r="292" spans="1:5" hidden="1">
       <c r="A292" s="2" t="s">
         <v>674</v>
       </c>
@@ -26174,7 +26313,7 @@
         <v>秋月型</v>
       </c>
     </row>
-    <row r="293" spans="1:5">
+    <row r="293" spans="1:5" hidden="1">
       <c r="A293" s="2" t="s">
         <v>675</v>
       </c>
@@ -26192,7 +26331,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="294" spans="1:5">
+    <row r="294" spans="1:5" hidden="1">
       <c r="A294" s="2" t="s">
         <v>676</v>
       </c>
@@ -26210,7 +26349,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="295" spans="1:5">
+    <row r="295" spans="1:5" hidden="1">
       <c r="A295" s="2" t="s">
         <v>677</v>
       </c>
@@ -26228,7 +26367,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="296" spans="1:5">
+    <row r="296" spans="1:5" hidden="1">
       <c r="A296" s="2" t="s">
         <v>678</v>
       </c>
@@ -26246,7 +26385,7 @@
         <v>球磨型</v>
       </c>
     </row>
-    <row r="297" spans="1:5">
+    <row r="297" spans="1:5" hidden="1">
       <c r="A297" s="2" t="s">
         <v>679</v>
       </c>
@@ -26264,7 +26403,7 @@
         <v>睦月型</v>
       </c>
     </row>
-    <row r="298" spans="1:5">
+    <row r="298" spans="1:5" hidden="1">
       <c r="A298" s="2" t="s">
         <v>680</v>
       </c>
@@ -26282,7 +26421,7 @@
         <v>日振型</v>
       </c>
     </row>
-    <row r="299" spans="1:5">
+    <row r="299" spans="1:5" hidden="1">
       <c r="A299" s="2" t="s">
         <v>681</v>
       </c>
@@ -26300,7 +26439,7 @@
         <v>日振型</v>
       </c>
     </row>
-    <row r="300" spans="1:5">
+    <row r="300" spans="1:5" hidden="1">
       <c r="A300" s="2" t="s">
         <v>682</v>
       </c>
@@ -26318,7 +26457,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="301" spans="1:5">
+    <row r="301" spans="1:5" hidden="1">
       <c r="A301" s="2" t="s">
         <v>683</v>
       </c>
@@ -26336,7 +26475,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="302" spans="1:5">
+    <row r="302" spans="1:5" hidden="1">
       <c r="A302" s="2" t="s">
         <v>684</v>
       </c>
@@ -26354,7 +26493,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="303" spans="1:5">
+    <row r="303" spans="1:5" hidden="1">
       <c r="A303" s="2" t="s">
         <v>685</v>
       </c>
@@ -26372,7 +26511,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="304" spans="1:5">
+    <row r="304" spans="1:5" hidden="1">
       <c r="A304" s="2" t="s">
         <v>686</v>
       </c>
@@ -26390,7 +26529,7 @@
         <v>J・C・バトラー級</v>
       </c>
     </row>
-    <row r="305" spans="1:5">
+    <row r="305" spans="1:5" hidden="1">
       <c r="A305" s="2" t="s">
         <v>687</v>
       </c>
@@ -26408,7 +26547,7 @@
         <v>Fletcher級</v>
       </c>
     </row>
-    <row r="306" spans="1:5">
+    <row r="306" spans="1:5" hidden="1">
       <c r="A306" s="2" t="s">
         <v>688</v>
       </c>
@@ -26426,7 +26565,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="307" spans="1:5">
+    <row r="307" spans="1:5" hidden="1">
       <c r="A307" s="2" t="s">
         <v>689</v>
       </c>
@@ -26444,7 +26583,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="308" spans="1:5">
+    <row r="308" spans="1:5" hidden="1">
       <c r="A308" s="2" t="s">
         <v>690</v>
       </c>
@@ -26462,7 +26601,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="309" spans="1:5">
+    <row r="309" spans="1:5" hidden="1">
       <c r="A309" s="2" t="s">
         <v>691</v>
       </c>
@@ -26480,7 +26619,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="310" spans="1:5">
+    <row r="310" spans="1:5" hidden="1">
       <c r="A310" s="2" t="s">
         <v>692</v>
       </c>
@@ -26498,7 +26637,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="311" spans="1:5">
+    <row r="311" spans="1:5" hidden="1">
       <c r="A311" s="2" t="s">
         <v>693</v>
       </c>
@@ -26516,7 +26655,7 @@
         <v>陽炎型</v>
       </c>
     </row>
-    <row r="312" spans="1:5">
+    <row r="312" spans="1:5" hidden="1">
       <c r="A312" s="2" t="s">
         <v>694</v>
       </c>
@@ -26534,7 +26673,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="313" spans="1:5">
+    <row r="313" spans="1:5" hidden="1">
       <c r="A313" s="2" t="s">
         <v>695</v>
       </c>
@@ -26552,7 +26691,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="314" spans="1:5">
+    <row r="314" spans="1:5" hidden="1">
       <c r="A314" s="2" t="s">
         <v>696</v>
       </c>
@@ -26570,7 +26709,7 @@
         <v>ゴトランド級</v>
       </c>
     </row>
-    <row r="315" spans="1:5">
+    <row r="315" spans="1:5" hidden="1">
       <c r="A315" s="2" t="s">
         <v>697</v>
       </c>
@@ -26588,7 +26727,7 @@
         <v>マエストラーレ級</v>
       </c>
     </row>
-    <row r="316" spans="1:5">
+    <row r="316" spans="1:5" hidden="1">
       <c r="A316" s="2" t="s">
         <v>698</v>
       </c>
@@ -26606,7 +26745,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="317" spans="1:5">
+    <row r="317" spans="1:5" hidden="1">
       <c r="A317" s="2" t="s">
         <v>699</v>
       </c>
@@ -26624,7 +26763,7 @@
         <v>ゴトランド級</v>
       </c>
     </row>
-    <row r="318" spans="1:5">
+    <row r="318" spans="1:5" hidden="1">
       <c r="A318" s="2" t="s">
         <v>700</v>
       </c>
@@ -26660,7 +26799,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="320" spans="1:5">
+    <row r="320" spans="1:5" hidden="1">
       <c r="A320" s="2" t="s">
         <v>702</v>
       </c>
@@ -26678,7 +26817,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="321" spans="1:5">
+    <row r="321" spans="1:5" hidden="1">
       <c r="A321" s="2" t="s">
         <v>703</v>
       </c>
@@ -26696,7 +26835,7 @@
         <v>占守型</v>
       </c>
     </row>
-    <row r="322" spans="1:5">
+    <row r="322" spans="1:5" hidden="1">
       <c r="A322" s="2" t="s">
         <v>704</v>
       </c>
@@ -26714,7 +26853,7 @@
         <v>改白露型</v>
       </c>
     </row>
-    <row r="323" spans="1:5">
+    <row r="323" spans="1:5" hidden="1">
       <c r="A323" s="2" t="s">
         <v>705</v>
       </c>
@@ -26732,7 +26871,7 @@
         <v>D・d・アブルッツィ級</v>
       </c>
     </row>
-    <row r="324" spans="1:5">
+    <row r="324" spans="1:5" hidden="1">
       <c r="A324" s="2" t="s">
         <v>706</v>
       </c>
@@ -26750,7 +26889,7 @@
         <v>D・d・アブルッツィ級</v>
       </c>
     </row>
-    <row r="325" spans="1:5">
+    <row r="325" spans="1:5" hidden="1">
       <c r="A325" s="2" t="s">
         <v>707</v>
       </c>
@@ -26768,7 +26907,7 @@
         <v>Fletcher級</v>
       </c>
     </row>
-    <row r="326" spans="1:5">
+    <row r="326" spans="1:5" hidden="1">
       <c r="A326" s="2" t="s">
         <v>708</v>
       </c>
@@ -26786,7 +26925,7 @@
         <v>アトランタ級</v>
       </c>
     </row>
-    <row r="327" spans="1:5">
+    <row r="327" spans="1:5" hidden="1">
       <c r="A327" s="2" t="s">
         <v>709</v>
       </c>
@@ -26804,7 +26943,7 @@
         <v>デ・ロイテル級</v>
       </c>
     </row>
-    <row r="328" spans="1:5">
+    <row r="328" spans="1:5" hidden="1">
       <c r="A328" s="2" t="s">
         <v>710</v>
       </c>
@@ -26822,7 +26961,7 @@
         <v>デ・ロイテル級</v>
       </c>
     </row>
-    <row r="329" spans="1:5">
+    <row r="329" spans="1:5" hidden="1">
       <c r="A329" s="2" t="s">
         <v>711</v>
       </c>
@@ -26840,7 +26979,7 @@
         <v>御蔵型</v>
       </c>
     </row>
-    <row r="330" spans="1:5">
+    <row r="330" spans="1:5" hidden="1">
       <c r="A330" s="2" t="s">
         <v>712</v>
       </c>
@@ -26858,7 +26997,7 @@
         <v>パース級</v>
       </c>
     </row>
-    <row r="331" spans="1:5">
+    <row r="331" spans="1:5" hidden="1">
       <c r="A331" s="2" t="s">
         <v>713</v>
       </c>
@@ -26876,7 +27015,7 @@
         <v>マエストラーレ級</v>
       </c>
     </row>
-    <row r="332" spans="1:5">
+    <row r="332" spans="1:5" hidden="1">
       <c r="A332" s="2" t="s">
         <v>714</v>
       </c>
@@ -26894,7 +27033,7 @@
         <v>御蔵型</v>
       </c>
     </row>
-    <row r="333" spans="1:5">
+    <row r="333" spans="1:5" hidden="1">
       <c r="A333" s="2" t="s">
         <v>715</v>
       </c>
@@ -26912,7 +27051,7 @@
         <v>パース級</v>
       </c>
     </row>
-    <row r="334" spans="1:5">
+    <row r="334" spans="1:5" hidden="1">
       <c r="A334" s="2" t="s">
         <v>716</v>
       </c>
@@ -26930,7 +27069,7 @@
         <v>マエストラーレ級</v>
       </c>
     </row>
-    <row r="335" spans="1:5">
+    <row r="335" spans="1:5" hidden="1">
       <c r="A335" s="2" t="s">
         <v>717</v>
       </c>
@@ -26948,7 +27087,7 @@
         <v>夕張型</v>
       </c>
     </row>
-    <row r="336" spans="1:5">
+    <row r="336" spans="1:5" hidden="1">
       <c r="A336" s="2" t="s">
         <v>718</v>
       </c>
@@ -26966,7 +27105,7 @@
         <v>夕張型</v>
       </c>
     </row>
-    <row r="337" spans="1:5">
+    <row r="337" spans="1:5" hidden="1">
       <c r="A337" s="2" t="s">
         <v>719</v>
       </c>
@@ -26984,7 +27123,7 @@
         <v>夕張型</v>
       </c>
     </row>
-    <row r="338" spans="1:5">
+    <row r="338" spans="1:5" hidden="1">
       <c r="A338" s="2" t="s">
         <v>720</v>
       </c>
@@ -27002,7 +27141,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="339" spans="1:5">
+    <row r="339" spans="1:5" hidden="1">
       <c r="A339" s="2" t="s">
         <v>721</v>
       </c>
@@ -27020,7 +27159,7 @@
         <v>綾波型</v>
       </c>
     </row>
-    <row r="340" spans="1:5">
+    <row r="340" spans="1:5" hidden="1">
       <c r="A340" s="2" t="s">
         <v>722</v>
       </c>
@@ -27038,7 +27177,7 @@
         <v>Fletcher級</v>
       </c>
     </row>
-    <row r="341" spans="1:5">
+    <row r="341" spans="1:5" hidden="1">
       <c r="A341" s="2" t="s">
         <v>723</v>
       </c>
@@ -27056,7 +27195,7 @@
         <v>改Fletcher級</v>
       </c>
     </row>
-    <row r="342" spans="1:5">
+    <row r="342" spans="1:5" hidden="1">
       <c r="A342" s="2" t="s">
         <v>724</v>
       </c>
@@ -27074,7 +27213,7 @@
         <v>ゴトランド級</v>
       </c>
     </row>
-    <row r="343" spans="1:5">
+    <row r="343" spans="1:5" hidden="1">
       <c r="A343" s="2" t="s">
         <v>725</v>
       </c>
@@ -27092,7 +27231,7 @@
         <v>日振型</v>
       </c>
     </row>
-    <row r="344" spans="1:5">
+    <row r="344" spans="1:5" hidden="1">
       <c r="A344" s="2" t="s">
         <v>726</v>
       </c>
@@ -27110,7 +27249,7 @@
         <v>日振型</v>
       </c>
     </row>
-    <row r="345" spans="1:5">
+    <row r="345" spans="1:5" hidden="1">
       <c r="A345" s="2" t="s">
         <v>727</v>
       </c>
@@ -27128,7 +27267,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="346" spans="1:5">
+    <row r="346" spans="1:5" hidden="1">
       <c r="A346" s="2" t="s">
         <v>728</v>
       </c>
@@ -27146,7 +27285,7 @@
         <v>J・C・バトラー級</v>
       </c>
     </row>
-    <row r="347" spans="1:5">
+    <row r="347" spans="1:5" hidden="1">
       <c r="A347" s="2" t="s">
         <v>729</v>
       </c>
@@ -27164,7 +27303,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="348" spans="1:5">
+    <row r="348" spans="1:5" hidden="1">
       <c r="A348" s="2" t="s">
         <v>730</v>
       </c>
@@ -27182,7 +27321,7 @@
         <v>択捉型</v>
       </c>
     </row>
-    <row r="349" spans="1:5">
+    <row r="349" spans="1:5" hidden="1">
       <c r="A349" s="2" t="s">
         <v>731</v>
       </c>
@@ -27218,7 +27357,7 @@
         <v>朝潮型</v>
       </c>
     </row>
-    <row r="351" spans="1:5">
+    <row r="351" spans="1:5" hidden="1">
       <c r="A351" s="2" t="s">
         <v>733</v>
       </c>
@@ -27236,7 +27375,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="352" spans="1:5">
+    <row r="352" spans="1:5" hidden="1">
       <c r="A352" s="2" t="s">
         <v>734</v>
       </c>
@@ -27254,7 +27393,7 @@
         <v>Fletcher級</v>
       </c>
     </row>
-    <row r="353" spans="1:5">
+    <row r="353" spans="1:5" hidden="1">
       <c r="A353" s="2" t="s">
         <v>735</v>
       </c>
@@ -27272,7 +27411,7 @@
         <v>D・d・アブルッツィ級</v>
       </c>
     </row>
-    <row r="354" spans="1:5">
+    <row r="354" spans="1:5" hidden="1">
       <c r="A354" s="2" t="s">
         <v>736</v>
       </c>
@@ -27290,7 +27429,7 @@
         <v>Fletcher級</v>
       </c>
     </row>
-    <row r="355" spans="1:5">
+    <row r="355" spans="1:5" hidden="1">
       <c r="A355" s="2" t="s">
         <v>737</v>
       </c>
@@ -27308,7 +27447,7 @@
         <v>D・d・アブルッツィ級</v>
       </c>
     </row>
-    <row r="356" spans="1:5">
+    <row r="356" spans="1:5" hidden="1">
       <c r="A356" s="2" t="s">
         <v>738</v>
       </c>
@@ -27326,7 +27465,7 @@
         <v>夕雲型</v>
       </c>
     </row>
-    <row r="357" spans="1:5">
+    <row r="357" spans="1:5" hidden="1">
       <c r="A357" s="2" t="s">
         <v>739</v>
       </c>
@@ -27344,7 +27483,7 @@
         <v>アトランタ級</v>
       </c>
     </row>
-    <row r="358" spans="1:5">
+    <row r="358" spans="1:5" hidden="1">
       <c r="A358" s="2" t="s">
         <v>740</v>
       </c>
@@ -27363,9 +27502,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C358" xr:uid="{A8194EA0-699C-439C-BDB5-7434AE4E38A1}"/>
+  <autoFilter ref="A1:E358" xr:uid="{A89E99B6-5863-4691-BB41-A8305AA2E545}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="朝潮型"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27373,13 +27519,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78BFAB31-BF52-42FA-85C6-00A20E51D9E4}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="3" max="3" width="26.125" customWidth="1"/>
+    <col min="3" max="3" width="26.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>